<commit_message>
finished w/ ddr dimm socket
</commit_message>
<xml_diff>
--- a/Excel Sheet/1GB DDR Mini DIMM 244.xlsx
+++ b/Excel Sheet/1GB DDR Mini DIMM 244.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="19320" windowHeight="9780" activeTab="2"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Capture Sorted'!$B$3:$I$247</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="270">
   <si>
     <t>VREF</t>
   </si>
@@ -505,6 +505,330 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>DU_139</t>
+  </si>
+  <si>
+    <t>DU_140</t>
+  </si>
+  <si>
+    <t>DU_224</t>
+  </si>
+  <si>
+    <t>DU_225</t>
+  </si>
+  <si>
+    <t>NC_19</t>
+  </si>
+  <si>
+    <t>NC_51</t>
+  </si>
+  <si>
+    <t>NC_56</t>
+  </si>
+  <si>
+    <t>NC_68</t>
+  </si>
+  <si>
+    <t>NC_80</t>
+  </si>
+  <si>
+    <t>NC_104</t>
+  </si>
+  <si>
+    <t>NC_128</t>
+  </si>
+  <si>
+    <t>NC_137</t>
+  </si>
+  <si>
+    <t>NC_149</t>
+  </si>
+  <si>
+    <t>NC_158</t>
+  </si>
+  <si>
+    <t>NC_167</t>
+  </si>
+  <si>
+    <t>NC_172</t>
+  </si>
+  <si>
+    <t>NC_201</t>
+  </si>
+  <si>
+    <t>NC_207</t>
+  </si>
+  <si>
+    <t>NC_216</t>
+  </si>
+  <si>
+    <t>NC_228</t>
+  </si>
+  <si>
+    <t>NC_237</t>
+  </si>
+  <si>
+    <t>VDD_54</t>
+  </si>
+  <si>
+    <t>VDD_60</t>
+  </si>
+  <si>
+    <t>VDD_65</t>
+  </si>
+  <si>
+    <t>VDD_69</t>
+  </si>
+  <si>
+    <t>VDD_72</t>
+  </si>
+  <si>
+    <t>VDD_74</t>
+  </si>
+  <si>
+    <t>VDD_175</t>
+  </si>
+  <si>
+    <t>VDD_181</t>
+  </si>
+  <si>
+    <t>VDD_187</t>
+  </si>
+  <si>
+    <t>VDD_190</t>
+  </si>
+  <si>
+    <t>VDD_193</t>
+  </si>
+  <si>
+    <t>VDD_200</t>
+  </si>
+  <si>
+    <t>VDDQ_52</t>
+  </si>
+  <si>
+    <t>VDDQ_57</t>
+  </si>
+  <si>
+    <t>VDDQ_63</t>
+  </si>
+  <si>
+    <t>VDDQ_76</t>
+  </si>
+  <si>
+    <t>VDDQ_79</t>
+  </si>
+  <si>
+    <t>VDDQ_173</t>
+  </si>
+  <si>
+    <t>VDDQ_178</t>
+  </si>
+  <si>
+    <t>VDDQ_184</t>
+  </si>
+  <si>
+    <t>VDDQ_195</t>
+  </si>
+  <si>
+    <t>VDDQ_197</t>
+  </si>
+  <si>
+    <t>VDDSPD_244</t>
+  </si>
+  <si>
+    <t>VSS_2</t>
+  </si>
+  <si>
+    <t>VSS_5</t>
+  </si>
+  <si>
+    <t>VSS_8</t>
+  </si>
+  <si>
+    <t>VSS_11</t>
+  </si>
+  <si>
+    <t>VSS_14</t>
+  </si>
+  <si>
+    <t>VSS_17</t>
+  </si>
+  <si>
+    <t>VSS_20</t>
+  </si>
+  <si>
+    <t>VSS_23</t>
+  </si>
+  <si>
+    <t>VSS_26</t>
+  </si>
+  <si>
+    <t>VSS_29</t>
+  </si>
+  <si>
+    <t>VSS_32</t>
+  </si>
+  <si>
+    <t>VSS_35</t>
+  </si>
+  <si>
+    <t>VSS_38</t>
+  </si>
+  <si>
+    <t>VSS_41</t>
+  </si>
+  <si>
+    <t>VSS_44</t>
+  </si>
+  <si>
+    <t>VSS_47</t>
+  </si>
+  <si>
+    <t>VSS_50</t>
+  </si>
+  <si>
+    <t>VSS_66</t>
+  </si>
+  <si>
+    <t>VSS_67</t>
+  </si>
+  <si>
+    <t>VSS_81</t>
+  </si>
+  <si>
+    <t>VSS_84</t>
+  </si>
+  <si>
+    <t>VSS_87</t>
+  </si>
+  <si>
+    <t>VSS_90</t>
+  </si>
+  <si>
+    <t>VSS_93</t>
+  </si>
+  <si>
+    <t>VSS_96</t>
+  </si>
+  <si>
+    <t>VSS_99</t>
+  </si>
+  <si>
+    <t>VSS_102</t>
+  </si>
+  <si>
+    <t>VSS_105</t>
+  </si>
+  <si>
+    <t>VSS_108</t>
+  </si>
+  <si>
+    <t>VSS_111</t>
+  </si>
+  <si>
+    <t>VSS_114</t>
+  </si>
+  <si>
+    <t>VSS_117</t>
+  </si>
+  <si>
+    <t>VSS_120</t>
+  </si>
+  <si>
+    <t>VSS_123</t>
+  </si>
+  <si>
+    <t>VSS_126</t>
+  </si>
+  <si>
+    <t>VSS_129</t>
+  </si>
+  <si>
+    <t>VSS_132</t>
+  </si>
+  <si>
+    <t>VSS_135</t>
+  </si>
+  <si>
+    <t>VSS_138</t>
+  </si>
+  <si>
+    <t>VSS_141</t>
+  </si>
+  <si>
+    <t>VSS_144</t>
+  </si>
+  <si>
+    <t>VSS_147</t>
+  </si>
+  <si>
+    <t>VSS_150</t>
+  </si>
+  <si>
+    <t>VSS_153</t>
+  </si>
+  <si>
+    <t>VSS_156</t>
+  </si>
+  <si>
+    <t>VSS_159</t>
+  </si>
+  <si>
+    <t>VSS_162</t>
+  </si>
+  <si>
+    <t>VSS_165</t>
+  </si>
+  <si>
+    <t>VSS_168</t>
+  </si>
+  <si>
+    <t>VSS_171</t>
+  </si>
+  <si>
+    <t>VSS_202</t>
+  </si>
+  <si>
+    <t>VSS_205</t>
+  </si>
+  <si>
+    <t>VSS_208</t>
+  </si>
+  <si>
+    <t>VSS_211</t>
+  </si>
+  <si>
+    <t>VSS_214</t>
+  </si>
+  <si>
+    <t>VSS_217</t>
+  </si>
+  <si>
+    <t>VSS_220</t>
+  </si>
+  <si>
+    <t>VSS_223</t>
+  </si>
+  <si>
+    <t>VSS_226</t>
+  </si>
+  <si>
+    <t>VSS_229</t>
+  </si>
+  <si>
+    <t>VSS_232</t>
+  </si>
+  <si>
+    <t>VSS_235</t>
+  </si>
+  <si>
+    <t>VSS_238</t>
+  </si>
+  <si>
+    <t>VSS_241</t>
   </si>
 </sst>
 </file>
@@ -4074,7 +4398,7 @@
   <dimension ref="B1:AS67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4251,7 +4575,7 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="M4" t="s">
         <v>152</v>
@@ -4287,7 +4611,7 @@
         <v>139</v>
       </c>
       <c r="AD4" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="AE4" t="s">
         <v>152</v>
@@ -4343,7 +4667,7 @@
         <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>4</v>
+        <v>207</v>
       </c>
       <c r="M5" t="s">
         <v>152</v>
@@ -4379,7 +4703,7 @@
         <v>140</v>
       </c>
       <c r="AD5" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="AE5" t="s">
         <v>152</v>
@@ -4435,7 +4759,7 @@
         <v>8</v>
       </c>
       <c r="L6" t="s">
-        <v>4</v>
+        <v>208</v>
       </c>
       <c r="M6" t="s">
         <v>152</v>
@@ -4450,10 +4774,10 @@
         <v>154</v>
       </c>
       <c r="T6">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="U6" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="V6" t="s">
         <v>152</v>
@@ -4471,7 +4795,7 @@
         <v>224</v>
       </c>
       <c r="AD6" t="s">
-        <v>61</v>
+        <v>164</v>
       </c>
       <c r="AE6" t="s">
         <v>152</v>
@@ -4527,7 +4851,7 @@
         <v>11</v>
       </c>
       <c r="L7" t="s">
-        <v>4</v>
+        <v>209</v>
       </c>
       <c r="M7" t="s">
         <v>152</v>
@@ -4542,10 +4866,10 @@
         <v>154</v>
       </c>
       <c r="T7">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="U7" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="V7" t="s">
         <v>152</v>
@@ -4563,7 +4887,7 @@
         <v>225</v>
       </c>
       <c r="AD7" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="AE7" t="s">
         <v>152</v>
@@ -4619,7 +4943,7 @@
         <v>14</v>
       </c>
       <c r="L8" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
       <c r="M8" t="s">
         <v>152</v>
@@ -4634,10 +4958,10 @@
         <v>154</v>
       </c>
       <c r="T8">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="U8" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="V8" t="s">
         <v>152</v>
@@ -4655,7 +4979,7 @@
         <v>19</v>
       </c>
       <c r="AD8" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="AE8" t="s">
         <v>152</v>
@@ -4711,7 +5035,7 @@
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
       <c r="M9" t="s">
         <v>152</v>
@@ -4726,10 +5050,10 @@
         <v>154</v>
       </c>
       <c r="T9">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="U9" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="V9" t="s">
         <v>152</v>
@@ -4747,7 +5071,7 @@
         <v>51</v>
       </c>
       <c r="AD9" t="s">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="AE9" t="s">
         <v>152</v>
@@ -4803,7 +5127,7 @@
         <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>4</v>
+        <v>212</v>
       </c>
       <c r="M10" t="s">
         <v>152</v>
@@ -4818,10 +5142,10 @@
         <v>154</v>
       </c>
       <c r="T10">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="U10" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="V10" t="s">
         <v>152</v>
@@ -4839,7 +5163,7 @@
         <v>56</v>
       </c>
       <c r="AD10" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
       <c r="AE10" t="s">
         <v>152</v>
@@ -4895,7 +5219,7 @@
         <v>23</v>
       </c>
       <c r="L11" t="s">
-        <v>4</v>
+        <v>213</v>
       </c>
       <c r="M11" t="s">
         <v>152</v>
@@ -4910,10 +5234,10 @@
         <v>154</v>
       </c>
       <c r="T11">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="U11" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="V11" t="s">
         <v>152</v>
@@ -4931,7 +5255,7 @@
         <v>68</v>
       </c>
       <c r="AD11" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="AE11" t="s">
         <v>152</v>
@@ -4987,7 +5311,7 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>4</v>
+        <v>214</v>
       </c>
       <c r="M12" t="s">
         <v>152</v>
@@ -5002,10 +5326,10 @@
         <v>154</v>
       </c>
       <c r="T12">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="U12" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="V12" t="s">
         <v>152</v>
@@ -5023,7 +5347,7 @@
         <v>80</v>
       </c>
       <c r="AD12" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="AE12" t="s">
         <v>152</v>
@@ -5079,7 +5403,7 @@
         <v>29</v>
       </c>
       <c r="L13" t="s">
-        <v>4</v>
+        <v>215</v>
       </c>
       <c r="M13" t="s">
         <v>152</v>
@@ -5094,10 +5418,10 @@
         <v>154</v>
       </c>
       <c r="T13">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="U13" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="V13" t="s">
         <v>152</v>
@@ -5115,7 +5439,7 @@
         <v>104</v>
       </c>
       <c r="AD13" t="s">
-        <v>27</v>
+        <v>171</v>
       </c>
       <c r="AE13" t="s">
         <v>152</v>
@@ -5171,7 +5495,7 @@
         <v>32</v>
       </c>
       <c r="L14" t="s">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="M14" t="s">
         <v>152</v>
@@ -5186,10 +5510,10 @@
         <v>154</v>
       </c>
       <c r="T14">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="U14" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="V14" t="s">
         <v>152</v>
@@ -5207,7 +5531,7 @@
         <v>128</v>
       </c>
       <c r="AD14" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="AE14" t="s">
         <v>152</v>
@@ -5263,7 +5587,7 @@
         <v>35</v>
       </c>
       <c r="L15" t="s">
-        <v>4</v>
+        <v>217</v>
       </c>
       <c r="M15" t="s">
         <v>152</v>
@@ -5278,10 +5602,10 @@
         <v>154</v>
       </c>
       <c r="T15">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="U15" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="V15" t="s">
         <v>152</v>
@@ -5299,7 +5623,7 @@
         <v>137</v>
       </c>
       <c r="AD15" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
       <c r="AE15" t="s">
         <v>152</v>
@@ -5355,7 +5679,7 @@
         <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="M16" t="s">
         <v>152</v>
@@ -5370,10 +5694,10 @@
         <v>154</v>
       </c>
       <c r="T16">
-        <v>9</v>
+        <v>133</v>
       </c>
       <c r="U16" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="V16" t="s">
         <v>152</v>
@@ -5391,7 +5715,7 @@
         <v>149</v>
       </c>
       <c r="AD16" t="s">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="AE16" t="s">
         <v>152</v>
@@ -5447,7 +5771,7 @@
         <v>41</v>
       </c>
       <c r="L17" t="s">
-        <v>4</v>
+        <v>219</v>
       </c>
       <c r="M17" t="s">
         <v>152</v>
@@ -5462,10 +5786,10 @@
         <v>154</v>
       </c>
       <c r="T17">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="U17" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="V17" t="s">
         <v>152</v>
@@ -5483,7 +5807,7 @@
         <v>158</v>
       </c>
       <c r="AD17" t="s">
-        <v>27</v>
+        <v>175</v>
       </c>
       <c r="AE17" t="s">
         <v>152</v>
@@ -5539,7 +5863,7 @@
         <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="M18" t="s">
         <v>152</v>
@@ -5554,10 +5878,10 @@
         <v>154</v>
       </c>
       <c r="T18">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="U18" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="V18" t="s">
         <v>152</v>
@@ -5575,7 +5899,7 @@
         <v>167</v>
       </c>
       <c r="AD18" t="s">
-        <v>27</v>
+        <v>176</v>
       </c>
       <c r="AE18" t="s">
         <v>152</v>
@@ -5631,7 +5955,7 @@
         <v>47</v>
       </c>
       <c r="L19" t="s">
-        <v>4</v>
+        <v>221</v>
       </c>
       <c r="M19" t="s">
         <v>152</v>
@@ -5646,10 +5970,10 @@
         <v>154</v>
       </c>
       <c r="T19">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="U19" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="V19" t="s">
         <v>152</v>
@@ -5667,7 +5991,7 @@
         <v>172</v>
       </c>
       <c r="AD19" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="AE19" t="s">
         <v>152</v>
@@ -5723,7 +6047,7 @@
         <v>50</v>
       </c>
       <c r="L20" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="M20" t="s">
         <v>152</v>
@@ -5738,10 +6062,10 @@
         <v>154</v>
       </c>
       <c r="T20">
-        <v>152</v>
+        <v>24</v>
       </c>
       <c r="U20" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="V20" t="s">
         <v>152</v>
@@ -5759,7 +6083,7 @@
         <v>201</v>
       </c>
       <c r="AD20" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="AE20" t="s">
         <v>152</v>
@@ -5815,7 +6139,7 @@
         <v>66</v>
       </c>
       <c r="L21" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
       <c r="M21" t="s">
         <v>152</v>
@@ -5830,10 +6154,10 @@
         <v>154</v>
       </c>
       <c r="T21">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="U21" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="V21" t="s">
         <v>152</v>
@@ -5851,7 +6175,7 @@
         <v>207</v>
       </c>
       <c r="AD21" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="AE21" t="s">
         <v>152</v>
@@ -5889,7 +6213,7 @@
         <v>67</v>
       </c>
       <c r="L22" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="M22" t="s">
         <v>152</v>
@@ -5904,10 +6228,10 @@
         <v>154</v>
       </c>
       <c r="T22">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="U22" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="V22" t="s">
         <v>152</v>
@@ -5925,7 +6249,7 @@
         <v>216</v>
       </c>
       <c r="AD22" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="AE22" t="s">
         <v>152</v>
@@ -5963,7 +6287,7 @@
         <v>81</v>
       </c>
       <c r="L23" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="M23" t="s">
         <v>152</v>
@@ -5978,10 +6302,10 @@
         <v>154</v>
       </c>
       <c r="T23">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="U23" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="V23" t="s">
         <v>152</v>
@@ -5999,7 +6323,7 @@
         <v>228</v>
       </c>
       <c r="AD23" t="s">
-        <v>27</v>
+        <v>181</v>
       </c>
       <c r="AE23" t="s">
         <v>152</v>
@@ -6037,7 +6361,7 @@
         <v>84</v>
       </c>
       <c r="L24" t="s">
-        <v>4</v>
+        <v>226</v>
       </c>
       <c r="M24" t="s">
         <v>152</v>
@@ -6052,10 +6376,10 @@
         <v>154</v>
       </c>
       <c r="T24">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="U24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="V24" t="s">
         <v>152</v>
@@ -6073,7 +6397,7 @@
         <v>237</v>
       </c>
       <c r="AD24" t="s">
-        <v>27</v>
+        <v>182</v>
       </c>
       <c r="AE24" t="s">
         <v>152</v>
@@ -6111,7 +6435,7 @@
         <v>87</v>
       </c>
       <c r="L25" t="s">
-        <v>4</v>
+        <v>227</v>
       </c>
       <c r="M25" t="s">
         <v>152</v>
@@ -6126,10 +6450,10 @@
         <v>154</v>
       </c>
       <c r="T25">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="U25" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="V25" t="s">
         <v>152</v>
@@ -6147,7 +6471,7 @@
         <v>54</v>
       </c>
       <c r="AD25" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="AE25" t="s">
         <v>152</v>
@@ -6185,7 +6509,7 @@
         <v>90</v>
       </c>
       <c r="L26" t="s">
-        <v>4</v>
+        <v>228</v>
       </c>
       <c r="M26" t="s">
         <v>152</v>
@@ -6200,10 +6524,10 @@
         <v>154</v>
       </c>
       <c r="T26">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="U26" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="V26" t="s">
         <v>152</v>
@@ -6221,7 +6545,7 @@
         <v>60</v>
       </c>
       <c r="AD26" t="s">
-        <v>6</v>
+        <v>184</v>
       </c>
       <c r="AE26" t="s">
         <v>152</v>
@@ -6259,7 +6583,7 @@
         <v>93</v>
       </c>
       <c r="L27" t="s">
-        <v>4</v>
+        <v>229</v>
       </c>
       <c r="M27" t="s">
         <v>152</v>
@@ -6274,10 +6598,10 @@
         <v>154</v>
       </c>
       <c r="T27">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="U27" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="V27" t="s">
         <v>152</v>
@@ -6295,7 +6619,7 @@
         <v>65</v>
       </c>
       <c r="AD27" t="s">
-        <v>6</v>
+        <v>185</v>
       </c>
       <c r="AE27" t="s">
         <v>152</v>
@@ -6333,7 +6657,7 @@
         <v>96</v>
       </c>
       <c r="L28" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="M28" t="s">
         <v>152</v>
@@ -6348,10 +6672,10 @@
         <v>154</v>
       </c>
       <c r="T28">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="U28" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="V28" t="s">
         <v>152</v>
@@ -6369,7 +6693,7 @@
         <v>69</v>
       </c>
       <c r="AD28" t="s">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="AE28" t="s">
         <v>152</v>
@@ -6407,7 +6731,7 @@
         <v>99</v>
       </c>
       <c r="L29" t="s">
-        <v>4</v>
+        <v>231</v>
       </c>
       <c r="M29" t="s">
         <v>152</v>
@@ -6422,10 +6746,10 @@
         <v>154</v>
       </c>
       <c r="T29">
-        <v>161</v>
+        <v>34</v>
       </c>
       <c r="U29" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="V29" t="s">
         <v>152</v>
@@ -6443,7 +6767,7 @@
         <v>72</v>
       </c>
       <c r="AD29" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="AE29" t="s">
         <v>152</v>
@@ -6481,7 +6805,7 @@
         <v>102</v>
       </c>
       <c r="L30" t="s">
-        <v>4</v>
+        <v>232</v>
       </c>
       <c r="M30" t="s">
         <v>152</v>
@@ -6496,10 +6820,10 @@
         <v>154</v>
       </c>
       <c r="T30">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="U30" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="V30" t="s">
         <v>152</v>
@@ -6517,7 +6841,7 @@
         <v>74</v>
       </c>
       <c r="AD30" t="s">
-        <v>6</v>
+        <v>188</v>
       </c>
       <c r="AE30" t="s">
         <v>152</v>
@@ -6555,7 +6879,7 @@
         <v>105</v>
       </c>
       <c r="L31" t="s">
-        <v>4</v>
+        <v>233</v>
       </c>
       <c r="M31" t="s">
         <v>152</v>
@@ -6570,10 +6894,10 @@
         <v>154</v>
       </c>
       <c r="T31">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="U31" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="V31" t="s">
         <v>152</v>
@@ -6591,7 +6915,7 @@
         <v>175</v>
       </c>
       <c r="AD31" t="s">
-        <v>6</v>
+        <v>189</v>
       </c>
       <c r="AE31" t="s">
         <v>152</v>
@@ -6629,7 +6953,7 @@
         <v>108</v>
       </c>
       <c r="L32" t="s">
-        <v>4</v>
+        <v>234</v>
       </c>
       <c r="M32" t="s">
         <v>152</v>
@@ -6644,10 +6968,10 @@
         <v>154</v>
       </c>
       <c r="T32">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="U32" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="V32" t="s">
         <v>152</v>
@@ -6665,7 +6989,7 @@
         <v>181</v>
       </c>
       <c r="AD32" t="s">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="AE32" t="s">
         <v>152</v>
@@ -6703,7 +7027,7 @@
         <v>111</v>
       </c>
       <c r="L33" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="M33" t="s">
         <v>152</v>
@@ -6718,10 +7042,10 @@
         <v>154</v>
       </c>
       <c r="T33">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="U33" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="V33" t="s">
         <v>152</v>
@@ -6739,7 +7063,7 @@
         <v>187</v>
       </c>
       <c r="AD33" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="AE33" t="s">
         <v>152</v>
@@ -6777,7 +7101,7 @@
         <v>114</v>
       </c>
       <c r="L34" t="s">
-        <v>4</v>
+        <v>236</v>
       </c>
       <c r="M34" t="s">
         <v>152</v>
@@ -6792,10 +7116,10 @@
         <v>154</v>
       </c>
       <c r="T34">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="U34" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="V34" t="s">
         <v>152</v>
@@ -6813,7 +7137,7 @@
         <v>190</v>
       </c>
       <c r="AD34" t="s">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="AE34" t="s">
         <v>152</v>
@@ -6851,7 +7175,7 @@
         <v>117</v>
       </c>
       <c r="L35" t="s">
-        <v>4</v>
+        <v>237</v>
       </c>
       <c r="M35" t="s">
         <v>152</v>
@@ -6866,10 +7190,10 @@
         <v>154</v>
       </c>
       <c r="T35">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="U35" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="V35" t="s">
         <v>152</v>
@@ -6887,7 +7211,7 @@
         <v>193</v>
       </c>
       <c r="AD35" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
       <c r="AE35" t="s">
         <v>152</v>
@@ -6925,7 +7249,7 @@
         <v>120</v>
       </c>
       <c r="L36" t="s">
-        <v>4</v>
+        <v>238</v>
       </c>
       <c r="M36" t="s">
         <v>152</v>
@@ -6940,10 +7264,10 @@
         <v>155</v>
       </c>
       <c r="T36">
-        <v>209</v>
+        <v>82</v>
       </c>
       <c r="U36" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="V36" t="s">
         <v>152</v>
@@ -6961,7 +7285,7 @@
         <v>200</v>
       </c>
       <c r="AD36" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="AE36" t="s">
         <v>152</v>
@@ -6999,7 +7323,7 @@
         <v>123</v>
       </c>
       <c r="L37" t="s">
-        <v>4</v>
+        <v>239</v>
       </c>
       <c r="M37" t="s">
         <v>152</v>
@@ -7014,10 +7338,10 @@
         <v>155</v>
       </c>
       <c r="T37">
-        <v>210</v>
+        <v>83</v>
       </c>
       <c r="U37" t="s">
-        <v>136</v>
+        <v>54</v>
       </c>
       <c r="V37" t="s">
         <v>152</v>
@@ -7035,7 +7359,7 @@
         <v>52</v>
       </c>
       <c r="AD37" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="AE37" t="s">
         <v>152</v>
@@ -7073,7 +7397,7 @@
         <v>126</v>
       </c>
       <c r="L38" t="s">
-        <v>4</v>
+        <v>240</v>
       </c>
       <c r="M38" t="s">
         <v>152</v>
@@ -7088,10 +7412,10 @@
         <v>155</v>
       </c>
       <c r="T38">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="U38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="V38" t="s">
         <v>152</v>
@@ -7109,7 +7433,7 @@
         <v>57</v>
       </c>
       <c r="AD38" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="AE38" t="s">
         <v>152</v>
@@ -7147,7 +7471,7 @@
         <v>129</v>
       </c>
       <c r="L39" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="M39" t="s">
         <v>152</v>
@@ -7162,10 +7486,10 @@
         <v>155</v>
       </c>
       <c r="T39">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="U39" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="V39" t="s">
         <v>152</v>
@@ -7183,7 +7507,7 @@
         <v>63</v>
       </c>
       <c r="AD39" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="AE39" t="s">
         <v>152</v>
@@ -7221,7 +7545,7 @@
         <v>132</v>
       </c>
       <c r="L40" t="s">
-        <v>4</v>
+        <v>242</v>
       </c>
       <c r="M40" t="s">
         <v>152</v>
@@ -7236,10 +7560,10 @@
         <v>155</v>
       </c>
       <c r="T40">
-        <v>92</v>
+        <v>203</v>
       </c>
       <c r="U40" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="V40" t="s">
         <v>152</v>
@@ -7257,7 +7581,7 @@
         <v>76</v>
       </c>
       <c r="AD40" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="AE40" t="s">
         <v>152</v>
@@ -7295,7 +7619,7 @@
         <v>135</v>
       </c>
       <c r="L41" t="s">
-        <v>4</v>
+        <v>243</v>
       </c>
       <c r="M41" t="s">
         <v>152</v>
@@ -7310,10 +7634,10 @@
         <v>155</v>
       </c>
       <c r="T41">
-        <v>97</v>
+        <v>204</v>
       </c>
       <c r="U41" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="V41" t="s">
         <v>152</v>
@@ -7331,7 +7655,7 @@
         <v>79</v>
       </c>
       <c r="AD41" t="s">
-        <v>13</v>
+        <v>199</v>
       </c>
       <c r="AE41" t="s">
         <v>152</v>
@@ -7369,7 +7693,7 @@
         <v>138</v>
       </c>
       <c r="L42" t="s">
-        <v>4</v>
+        <v>244</v>
       </c>
       <c r="M42" t="s">
         <v>152</v>
@@ -7384,10 +7708,10 @@
         <v>155</v>
       </c>
       <c r="T42">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="U42" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="V42" t="s">
         <v>152</v>
@@ -7405,7 +7729,7 @@
         <v>173</v>
       </c>
       <c r="AD42" t="s">
-        <v>13</v>
+        <v>200</v>
       </c>
       <c r="AE42" t="s">
         <v>152</v>
@@ -7443,7 +7767,7 @@
         <v>141</v>
       </c>
       <c r="L43" t="s">
-        <v>4</v>
+        <v>245</v>
       </c>
       <c r="M43" t="s">
         <v>152</v>
@@ -7458,10 +7782,10 @@
         <v>155</v>
       </c>
       <c r="T43">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="U43" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
       <c r="V43" t="s">
         <v>152</v>
@@ -7479,7 +7803,7 @@
         <v>178</v>
       </c>
       <c r="AD43" t="s">
-        <v>13</v>
+        <v>201</v>
       </c>
       <c r="AE43" t="s">
         <v>152</v>
@@ -7517,7 +7841,7 @@
         <v>144</v>
       </c>
       <c r="L44" t="s">
-        <v>4</v>
+        <v>246</v>
       </c>
       <c r="M44" t="s">
         <v>152</v>
@@ -7532,10 +7856,10 @@
         <v>155</v>
       </c>
       <c r="T44">
-        <v>213</v>
+        <v>91</v>
       </c>
       <c r="U44" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="V44" t="s">
         <v>152</v>
@@ -7553,7 +7877,7 @@
         <v>184</v>
       </c>
       <c r="AD44" t="s">
-        <v>13</v>
+        <v>202</v>
       </c>
       <c r="AE44" t="s">
         <v>152</v>
@@ -7591,7 +7915,7 @@
         <v>147</v>
       </c>
       <c r="L45" t="s">
-        <v>4</v>
+        <v>247</v>
       </c>
       <c r="M45" t="s">
         <v>152</v>
@@ -7606,10 +7930,10 @@
         <v>155</v>
       </c>
       <c r="T45">
-        <v>218</v>
+        <v>92</v>
       </c>
       <c r="U45" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="V45" t="s">
         <v>152</v>
@@ -7627,7 +7951,7 @@
         <v>195</v>
       </c>
       <c r="AD45" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="AE45" t="s">
         <v>152</v>
@@ -7665,7 +7989,7 @@
         <v>150</v>
       </c>
       <c r="L46" t="s">
-        <v>4</v>
+        <v>248</v>
       </c>
       <c r="M46" t="s">
         <v>152</v>
@@ -7680,10 +8004,10 @@
         <v>155</v>
       </c>
       <c r="T46">
-        <v>219</v>
+        <v>97</v>
       </c>
       <c r="U46" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="V46" t="s">
         <v>152</v>
@@ -7701,7 +8025,7 @@
         <v>197</v>
       </c>
       <c r="AD46" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="AE46" t="s">
         <v>152</v>
@@ -7739,7 +8063,7 @@
         <v>153</v>
       </c>
       <c r="L47" t="s">
-        <v>4</v>
+        <v>249</v>
       </c>
       <c r="M47" t="s">
         <v>152</v>
@@ -7754,10 +8078,10 @@
         <v>155</v>
       </c>
       <c r="T47">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U47" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="V47" t="s">
         <v>152</v>
@@ -7775,7 +8099,7 @@
         <v>244</v>
       </c>
       <c r="AD47" t="s">
-        <v>134</v>
+        <v>205</v>
       </c>
       <c r="AE47" t="s">
         <v>152</v>
@@ -7813,7 +8137,7 @@
         <v>156</v>
       </c>
       <c r="L48" t="s">
-        <v>4</v>
+        <v>250</v>
       </c>
       <c r="M48" t="s">
         <v>152</v>
@@ -7828,10 +8152,10 @@
         <v>155</v>
       </c>
       <c r="T48">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="U48" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="V48" t="s">
         <v>152</v>
@@ -7887,7 +8211,7 @@
         <v>159</v>
       </c>
       <c r="L49" t="s">
-        <v>4</v>
+        <v>251</v>
       </c>
       <c r="M49" t="s">
         <v>152</v>
@@ -7902,10 +8226,10 @@
         <v>155</v>
       </c>
       <c r="T49">
-        <v>125</v>
+        <v>213</v>
       </c>
       <c r="U49" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="V49" t="s">
         <v>152</v>
@@ -7943,7 +8267,7 @@
         <v>162</v>
       </c>
       <c r="L50" t="s">
-        <v>4</v>
+        <v>252</v>
       </c>
       <c r="M50" t="s">
         <v>152</v>
@@ -7958,10 +8282,10 @@
         <v>155</v>
       </c>
       <c r="T50">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="U50" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="V50" t="s">
         <v>152</v>
@@ -7999,7 +8323,7 @@
         <v>165</v>
       </c>
       <c r="L51" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
       <c r="M51" t="s">
         <v>152</v>
@@ -8014,10 +8338,10 @@
         <v>155</v>
       </c>
       <c r="T51">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="U51" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="V51" t="s">
         <v>152</v>
@@ -8055,7 +8379,7 @@
         <v>168</v>
       </c>
       <c r="L52" t="s">
-        <v>4</v>
+        <v>254</v>
       </c>
       <c r="M52" t="s">
         <v>152</v>
@@ -8070,10 +8394,10 @@
         <v>155</v>
       </c>
       <c r="T52">
-        <v>221</v>
+        <v>100</v>
       </c>
       <c r="U52" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="V52" t="s">
         <v>152</v>
@@ -8111,7 +8435,7 @@
         <v>171</v>
       </c>
       <c r="L53" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="M53" t="s">
         <v>152</v>
@@ -8126,10 +8450,10 @@
         <v>155</v>
       </c>
       <c r="T53">
-        <v>222</v>
+        <v>101</v>
       </c>
       <c r="U53" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="V53" t="s">
         <v>152</v>
@@ -8167,7 +8491,7 @@
         <v>202</v>
       </c>
       <c r="L54" t="s">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="M54" t="s">
         <v>152</v>
@@ -8182,10 +8506,10 @@
         <v>155</v>
       </c>
       <c r="T54">
-        <v>230</v>
+        <v>109</v>
       </c>
       <c r="U54" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="V54" t="s">
         <v>152</v>
@@ -8223,7 +8547,7 @@
         <v>205</v>
       </c>
       <c r="L55" t="s">
-        <v>4</v>
+        <v>257</v>
       </c>
       <c r="M55" t="s">
         <v>152</v>
@@ -8238,10 +8562,10 @@
         <v>155</v>
       </c>
       <c r="T55">
-        <v>231</v>
+        <v>110</v>
       </c>
       <c r="U55" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="V55" t="s">
         <v>152</v>
@@ -8279,7 +8603,7 @@
         <v>208</v>
       </c>
       <c r="L56" t="s">
-        <v>4</v>
+        <v>258</v>
       </c>
       <c r="M56" t="s">
         <v>152</v>
@@ -8294,10 +8618,10 @@
         <v>155</v>
       </c>
       <c r="T56">
-        <v>112</v>
+        <v>221</v>
       </c>
       <c r="U56" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="V56" t="s">
         <v>152</v>
@@ -8335,7 +8659,7 @@
         <v>211</v>
       </c>
       <c r="L57" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="M57" t="s">
         <v>152</v>
@@ -8350,10 +8674,10 @@
         <v>155</v>
       </c>
       <c r="T57">
-        <v>113</v>
+        <v>222</v>
       </c>
       <c r="U57" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="V57" t="s">
         <v>152</v>
@@ -8373,7 +8697,7 @@
         <v>214</v>
       </c>
       <c r="L58" t="s">
-        <v>4</v>
+        <v>260</v>
       </c>
       <c r="M58" t="s">
         <v>152</v>
@@ -8388,10 +8712,10 @@
         <v>155</v>
       </c>
       <c r="T58">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="U58" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="V58" t="s">
         <v>152</v>
@@ -8411,7 +8735,7 @@
         <v>217</v>
       </c>
       <c r="L59" t="s">
-        <v>4</v>
+        <v>261</v>
       </c>
       <c r="M59" t="s">
         <v>152</v>
@@ -8426,10 +8750,10 @@
         <v>155</v>
       </c>
       <c r="T59">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="U59" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="V59" t="s">
         <v>152</v>
@@ -8449,7 +8773,7 @@
         <v>220</v>
       </c>
       <c r="L60" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="M60" t="s">
         <v>152</v>
@@ -8464,10 +8788,10 @@
         <v>155</v>
       </c>
       <c r="T60">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="U60" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="V60" t="s">
         <v>152</v>
@@ -8487,7 +8811,7 @@
         <v>223</v>
       </c>
       <c r="L61" t="s">
-        <v>4</v>
+        <v>263</v>
       </c>
       <c r="M61" t="s">
         <v>152</v>
@@ -8502,10 +8826,10 @@
         <v>155</v>
       </c>
       <c r="T61">
-        <v>233</v>
+        <v>113</v>
       </c>
       <c r="U61" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="V61" t="s">
         <v>152</v>
@@ -8525,7 +8849,7 @@
         <v>226</v>
       </c>
       <c r="L62" t="s">
-        <v>4</v>
+        <v>264</v>
       </c>
       <c r="M62" t="s">
         <v>152</v>
@@ -8540,10 +8864,10 @@
         <v>155</v>
       </c>
       <c r="T62">
-        <v>234</v>
+        <v>118</v>
       </c>
       <c r="U62" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="V62" t="s">
         <v>152</v>
@@ -8563,7 +8887,7 @@
         <v>229</v>
       </c>
       <c r="L63" t="s">
-        <v>4</v>
+        <v>265</v>
       </c>
       <c r="M63" t="s">
         <v>152</v>
@@ -8578,10 +8902,10 @@
         <v>155</v>
       </c>
       <c r="T63">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="U63" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="V63" t="s">
         <v>152</v>
@@ -8601,7 +8925,7 @@
         <v>232</v>
       </c>
       <c r="L64" t="s">
-        <v>4</v>
+        <v>266</v>
       </c>
       <c r="M64" t="s">
         <v>152</v>
@@ -8616,10 +8940,10 @@
         <v>155</v>
       </c>
       <c r="T64">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="U64" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="V64" t="s">
         <v>152</v>
@@ -8639,7 +8963,7 @@
         <v>235</v>
       </c>
       <c r="L65" t="s">
-        <v>4</v>
+        <v>267</v>
       </c>
       <c r="M65" t="s">
         <v>152</v>
@@ -8654,10 +8978,10 @@
         <v>155</v>
       </c>
       <c r="T65">
-        <v>131</v>
+        <v>234</v>
       </c>
       <c r="U65" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="V65" t="s">
         <v>152</v>
@@ -8677,7 +9001,7 @@
         <v>238</v>
       </c>
       <c r="L66" t="s">
-        <v>4</v>
+        <v>268</v>
       </c>
       <c r="M66" t="s">
         <v>152</v>
@@ -8692,10 +9016,10 @@
         <v>155</v>
       </c>
       <c r="T66">
-        <v>12</v>
+        <v>239</v>
       </c>
       <c r="U66" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="V66" t="s">
         <v>152</v>
@@ -8715,7 +9039,7 @@
         <v>241</v>
       </c>
       <c r="L67" t="s">
-        <v>4</v>
+        <v>269</v>
       </c>
       <c r="M67" t="s">
         <v>152</v>
@@ -8730,10 +9054,10 @@
         <v>155</v>
       </c>
       <c r="T67">
-        <v>13</v>
+        <v>240</v>
       </c>
       <c r="U67" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="V67" t="s">
         <v>152</v>
@@ -8749,6 +9073,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="S4:AA67">
+    <sortCondition ref="S4:S67"/>
+  </sortState>
   <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="K2:L2"/>

</xml_diff>